<commit_message>
put ! in logical group, update precedence numbers
</commit_message>
<xml_diff>
--- a/cpp_operator_precedence_by_group.xlsx
+++ b/cpp_operator_precedence_by_group.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26731"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{0DECEAC9-FDFD-49F0-A22C-3591A8C44117}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC260D87-31A1-463E-ABCF-63CC4F407490}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14880" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2730" yWindow="45" windowWidth="17820" windowHeight="15555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Invoice" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="ColumnTitle1">Invoice!$B$2:$E$11</definedName>
+    <definedName name="ColumnTitle1">Invoice!$B$2:$E$12</definedName>
     <definedName name="company_name">Invoice!$B$1</definedName>
     <definedName name="RowTitleRegion1..C7">Invoice!#REF!</definedName>
     <definedName name="RowTitleRegion2..G5">Invoice!#REF!</definedName>
@@ -42,9 +42,6 @@
     <t>first</t>
   </si>
   <si>
-    <t>unary operators</t>
-  </si>
-  <si>
     <t>second</t>
   </si>
   <si>
@@ -57,9 +54,6 @@
     <t xml:space="preserve"> *, /, %</t>
   </si>
   <si>
-    <t xml:space="preserve"> !, +, -</t>
-  </si>
-  <si>
     <t xml:space="preserve"> ()</t>
   </si>
   <si>
@@ -75,12 +69,6 @@
     <t>relational operators</t>
   </si>
   <si>
-    <t>arithmetic operators</t>
-  </si>
-  <si>
-    <t>fifth</t>
-  </si>
-  <si>
     <t xml:space="preserve"> ==, !=</t>
   </si>
   <si>
@@ -112,6 +100,18 @@
   </si>
   <si>
     <t>Group Precedence</t>
+  </si>
+  <si>
+    <t>math operators</t>
+  </si>
+  <si>
+    <t>unary minus sign that indicates a negative number like -1, -22, etc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> !</t>
+  </si>
+  <si>
+    <t>When  you see more than one operator with the same precedence, evaluate Left to Right.</t>
   </si>
 </sst>
 </file>
@@ -120,10 +120,10 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="#_)"/>
-    <numFmt numFmtId="166" formatCode="[&lt;=9999999]###\-####;\(###\)\ ###\-####"/>
+    <numFmt numFmtId="164" formatCode="#_)"/>
+    <numFmt numFmtId="165" formatCode="[&lt;=9999999]###\-####;\(###\)\ ###\-####"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="2" tint="-0.749961851863155"/>
@@ -235,8 +235,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="14">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -299,12 +307,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF5F5BF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -316,7 +318,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -398,6 +400,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFill="0" applyBorder="0">
@@ -440,17 +462,17 @@
     <xf numFmtId="0" fontId="14" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -460,7 +482,7 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -469,16 +491,7 @@
     <xf numFmtId="0" fontId="15" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="165" fontId="15" fillId="10" borderId="5" xfId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="15" fillId="11" borderId="5" xfId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="15" fillId="10" borderId="5" xfId="17" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -505,38 +518,53 @@
     <xf numFmtId="0" fontId="15" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="165" fontId="15" fillId="7" borderId="1" xfId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="15" fillId="7" borderId="1" xfId="17" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="15" fillId="5" borderId="5" xfId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="5" borderId="5" xfId="17" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="15" fillId="9" borderId="5" xfId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="9" borderId="5" xfId="17" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="164" fontId="15" fillId="8" borderId="5" xfId="17" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="165" fontId="15" fillId="8" borderId="5" xfId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -977,17 +1005,17 @@
     <tabColor theme="4" tint="-0.499984740745262"/>
     <pageSetUpPr autoPageBreaks="0" fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.42578125" customWidth="1"/>
     <col min="2" max="2" width="18.28515625" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" customWidth="1"/>
+    <col min="3" max="3" width="45.42578125" customWidth="1"/>
     <col min="4" max="4" width="30" customWidth="1"/>
     <col min="5" max="5" width="16.5703125" customWidth="1"/>
     <col min="6" max="6" width="11.28515625" customWidth="1"/>
@@ -995,25 +1023,25 @@
   <sheetData>
     <row r="1" spans="1:6" ht="57.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
     </row>
     <row r="2" spans="1:6" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E2" s="27" t="s">
-        <v>25</v>
+        <v>19</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="F2" s="1"/>
     </row>
@@ -1025,10 +1053,10 @@
         <v>1</v>
       </c>
       <c r="C3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>8</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>10</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>1</v>
@@ -1043,13 +1071,13 @@
         <v>2</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="18" t="s">
         <v>2</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>3</v>
       </c>
       <c r="F4" s="1"/>
     </row>
@@ -1057,49 +1085,45 @@
       <c r="A5">
         <v>3</v>
       </c>
-      <c r="B5" s="10">
+      <c r="B5" s="7">
         <v>3</v>
       </c>
-      <c r="C5" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="21" t="s">
-        <v>4</v>
-      </c>
+      <c r="C5" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="26"/>
+      <c r="E5" s="24"/>
       <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:6" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
-      <c r="B6" s="10">
+      <c r="B6" s="7">
         <v>4</v>
       </c>
-      <c r="C6" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="20"/>
-      <c r="E6" s="22"/>
+      <c r="C6" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="27"/>
+      <c r="E6" s="19"/>
       <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:6" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
-      <c r="B7" s="12">
+      <c r="B7" s="9">
         <v>5</v>
       </c>
-      <c r="C7" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="23" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" s="24" t="s">
+      <c r="C7" s="10" t="s">
         <v>9</v>
+      </c>
+      <c r="D7" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="21" t="s">
+        <v>3</v>
       </c>
       <c r="F7" s="1"/>
     </row>
@@ -1107,75 +1131,98 @@
       <c r="A8">
         <v>6</v>
       </c>
-      <c r="B8" s="12">
+      <c r="B8" s="9">
         <v>6</v>
       </c>
-      <c r="C8" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="20"/>
-      <c r="E8" s="22"/>
+      <c r="C8" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="17"/>
+      <c r="E8" s="19"/>
       <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:6" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9">
+        <v>2</v>
+      </c>
+      <c r="B9" s="11">
         <v>7</v>
       </c>
-      <c r="B9" s="14">
+      <c r="C9" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="22" t="s">
         <v>7</v>
-      </c>
-      <c r="C9" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="E9" s="26" t="s">
-        <v>14</v>
       </c>
       <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:6" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10">
+        <v>7</v>
+      </c>
+      <c r="B10" s="11">
         <v>8</v>
       </c>
-      <c r="B10" s="14">
-        <v>8</v>
-      </c>
-      <c r="C10" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" s="20"/>
-      <c r="E10" s="22"/>
+      <c r="C10" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="26"/>
+      <c r="E10" s="24"/>
       <c r="F10" s="1"/>
     </row>
     <row r="11" spans="1:6" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11">
+        <v>8</v>
+      </c>
+      <c r="B11" s="11">
         <v>9</v>
       </c>
-      <c r="B11" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="E11" s="18" t="s">
-        <v>21</v>
-      </c>
+      <c r="C11" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="27"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="1"/>
+    </row>
+    <row r="12" spans="1:6" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>9</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="30"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="30"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" selectLockedCells="1" sort="0"/>
-  <mergeCells count="7">
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
+  <mergeCells count="8">
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="E4:E6"/>
+    <mergeCell ref="D4:D6"/>
+    <mergeCell ref="D9:D11"/>
+    <mergeCell ref="E9:E11"/>
     <mergeCell ref="D7:D8"/>
     <mergeCell ref="E7:E8"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="B1:E1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations xWindow="760" yWindow="637" count="5">

</xml_diff>